<commit_message>
Add correct input Excel file
Uploaded Excel file with correct labels for fecundity figures
</commit_message>
<xml_diff>
--- a/cisco.xlsx
+++ b/cisco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/laura_lee_fws_gov/Documents/Documents/Git/USFWS GitHub/pva-lake-erie-cisco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="658" documentId="8_{29CC0380-1B16-48C8-8689-67AA598726F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEA7C6D5-C4B9-4BDB-A6A0-A7211A8737ED}"/>
+  <xr:revisionPtr revIDLastSave="661" documentId="8_{29CC0380-1B16-48C8-8689-67AA598726F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{991542F2-0F0F-4D50-87D0-887E78EA032F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="5" xr2:uid="{D2E97B22-AF74-4F08-A3D1-0F361F02F459}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="6" xr2:uid="{D2E97B22-AF74-4F08-A3D1-0F361F02F459}"/>
   </bookViews>
   <sheets>
     <sheet name="lw" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="35">
   <si>
     <t>age</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>weight</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Ontario</t>
   </si>
   <si>
     <t>Superior</t>
@@ -245,6 +239,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,13 +553,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -572,7 +570,7 @@
         <v>3.3487610000000001</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -583,7 +581,7 @@
         <v>3.4220429999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -594,7 +592,7 @@
         <v>3.344452</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -605,7 +603,7 @@
         <v>3.327674</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -616,7 +614,7 @@
         <v>3.1251069999999999</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -649,7 +647,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -660,7 +658,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -671,7 +669,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>140</v>
@@ -682,7 +680,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>160</v>
@@ -693,7 +691,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>180</v>
@@ -704,7 +702,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>200</v>
@@ -715,7 +713,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>220</v>
@@ -726,7 +724,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>240</v>
@@ -737,7 +735,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>260</v>
@@ -748,7 +746,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>280</v>
@@ -759,7 +757,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>300</v>
@@ -770,7 +768,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>320</v>
@@ -781,7 +779,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>340</v>
@@ -792,7 +790,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>360</v>
@@ -803,7 +801,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>380</v>
@@ -814,7 +812,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>400</v>
@@ -825,7 +823,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>420</v>
@@ -836,7 +834,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>440</v>
@@ -847,7 +845,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>460</v>
@@ -858,7 +856,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>480</v>
@@ -869,7 +867,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>500</v>
@@ -880,7 +878,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -891,7 +889,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>120</v>
@@ -902,7 +900,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>140</v>
@@ -913,7 +911,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>160</v>
@@ -924,7 +922,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>180</v>
@@ -935,7 +933,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>200</v>
@@ -946,7 +944,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <v>220</v>
@@ -957,7 +955,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30">
         <v>240</v>
@@ -968,7 +966,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <v>260</v>
@@ -979,7 +977,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>280</v>
@@ -990,7 +988,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>300</v>
@@ -1001,7 +999,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34">
         <v>320</v>
@@ -1012,7 +1010,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>340</v>
@@ -1023,7 +1021,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36">
         <v>360</v>
@@ -1034,7 +1032,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <v>380</v>
@@ -1045,7 +1043,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38">
         <v>400</v>
@@ -1056,7 +1054,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39">
         <v>420</v>
@@ -1067,7 +1065,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40">
         <v>440</v>
@@ -1078,7 +1076,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41">
         <v>460</v>
@@ -1089,7 +1087,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <v>480</v>
@@ -1100,7 +1098,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>500</v>
@@ -1111,7 +1109,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44">
         <v>100</v>
@@ -1122,7 +1120,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B45">
         <v>120</v>
@@ -1133,7 +1131,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46">
         <v>140</v>
@@ -1144,7 +1142,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B47">
         <v>160</v>
@@ -1155,7 +1153,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B48">
         <v>180</v>
@@ -1166,7 +1164,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49">
         <v>200</v>
@@ -1177,7 +1175,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50">
         <v>220</v>
@@ -1188,7 +1186,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B51">
         <v>240</v>
@@ -1199,7 +1197,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B52">
         <v>260</v>
@@ -1210,7 +1208,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53">
         <v>280</v>
@@ -1221,7 +1219,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B54">
         <v>300</v>
@@ -1232,7 +1230,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B55">
         <v>320</v>
@@ -1243,7 +1241,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B56">
         <v>340</v>
@@ -1254,7 +1252,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57">
         <v>360</v>
@@ -1265,7 +1263,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B58">
         <v>380</v>
@@ -1276,7 +1274,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59">
         <v>400</v>
@@ -1287,7 +1285,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B60">
         <v>420</v>
@@ -1298,7 +1296,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61">
         <v>440</v>
@@ -1309,7 +1307,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B62">
         <v>460</v>
@@ -1320,7 +1318,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B63">
         <v>480</v>
@@ -1331,7 +1329,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B64">
         <v>500</v>
@@ -1342,7 +1340,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -1353,7 +1351,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B66">
         <v>120</v>
@@ -1364,7 +1362,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B67">
         <v>140</v>
@@ -1375,7 +1373,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B68">
         <v>160</v>
@@ -1386,7 +1384,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B69">
         <v>180</v>
@@ -1397,7 +1395,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B70">
         <v>200</v>
@@ -1408,7 +1406,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B71">
         <v>220</v>
@@ -1419,7 +1417,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B72">
         <v>240</v>
@@ -1430,7 +1428,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B73">
         <v>260</v>
@@ -1441,7 +1439,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B74">
         <v>280</v>
@@ -1452,7 +1450,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B75">
         <v>300</v>
@@ -1463,7 +1461,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B76">
         <v>320</v>
@@ -1474,7 +1472,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B77">
         <v>340</v>
@@ -1485,7 +1483,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B78">
         <v>360</v>
@@ -1496,7 +1494,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B79">
         <v>380</v>
@@ -1507,7 +1505,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B80">
         <v>400</v>
@@ -1518,7 +1516,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B81">
         <v>420</v>
@@ -1529,7 +1527,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B82">
         <v>440</v>
@@ -1540,7 +1538,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B83">
         <v>460</v>
@@ -1551,7 +1549,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B84">
         <v>480</v>
@@ -1562,7 +1560,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B85">
         <v>500</v>
@@ -1573,7 +1571,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B86">
         <v>100</v>
@@ -1584,7 +1582,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B87">
         <v>120</v>
@@ -1595,7 +1593,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B88">
         <v>140</v>
@@ -1606,7 +1604,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B89">
         <v>160</v>
@@ -1617,7 +1615,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B90">
         <v>180</v>
@@ -1628,7 +1626,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B91">
         <v>200</v>
@@ -1639,7 +1637,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B92">
         <v>220</v>
@@ -1650,7 +1648,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B93">
         <v>240</v>
@@ -1661,7 +1659,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B94">
         <v>260</v>
@@ -1672,7 +1670,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B95">
         <v>280</v>
@@ -1683,7 +1681,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B96">
         <v>300</v>
@@ -1694,7 +1692,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B97">
         <v>320</v>
@@ -1705,7 +1703,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B98">
         <v>340</v>
@@ -1716,7 +1714,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B99">
         <v>360</v>
@@ -1727,7 +1725,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B100">
         <v>380</v>
@@ -1738,7 +1736,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B101">
         <v>400</v>
@@ -1749,7 +1747,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B102">
         <v>420</v>
@@ -1760,7 +1758,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B103">
         <v>440</v>
@@ -1771,7 +1769,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B104">
         <v>460</v>
@@ -1782,7 +1780,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B105">
         <v>480</v>
@@ -1793,7 +1791,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B106">
         <v>500</v>
@@ -1821,16 +1819,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1844,7 +1842,7 @@
         <v>-1.4911000000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1858,7 +1856,7 @@
         <v>-2.4512100000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1872,7 +1870,7 @@
         <v>-1.70448</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1886,7 +1884,7 @@
         <v>-1.8246</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1900,7 +1898,7 @@
         <v>-3.2610000000000001</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1919,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1932,7 +1930,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1943,7 +1941,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -1954,7 +1952,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1965,7 +1963,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -1976,7 +1974,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -1987,7 +1985,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -1998,7 +1996,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -2009,7 +2007,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -2020,7 +2018,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -2031,7 +2029,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -2042,7 +2040,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -2053,7 +2051,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -2064,7 +2062,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -2075,7 +2073,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -2086,7 +2084,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -2097,7 +2095,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -2108,7 +2106,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
@@ -2119,7 +2117,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -2130,7 +2128,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>4</v>
@@ -2141,7 +2139,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>5</v>
@@ -2152,7 +2150,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2">
         <v>6</v>
@@ -2163,7 +2161,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
         <v>7</v>
@@ -2174,7 +2172,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2">
         <v>8</v>
@@ -2185,7 +2183,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2">
         <v>9</v>
@@ -2196,7 +2194,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2">
         <v>10</v>
@@ -2207,7 +2205,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2">
         <v>11</v>
@@ -2218,7 +2216,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2">
         <v>12</v>
@@ -2229,7 +2227,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2">
         <v>13</v>
@@ -2240,7 +2238,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2">
         <v>14</v>
@@ -2251,7 +2249,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B31" s="2">
         <v>15</v>
@@ -2262,7 +2260,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
@@ -2273,7 +2271,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" s="2">
         <v>2</v>
@@ -2284,7 +2282,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" s="2">
         <v>3</v>
@@ -2295,7 +2293,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" s="2">
         <v>4</v>
@@ -2306,7 +2304,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2">
         <v>5</v>
@@ -2317,7 +2315,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B37" s="2">
         <v>6</v>
@@ -2328,7 +2326,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" s="2">
         <v>7</v>
@@ -2339,7 +2337,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B39" s="2">
         <v>8</v>
@@ -2350,7 +2348,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B40" s="2">
         <v>9</v>
@@ -2361,7 +2359,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B41" s="2">
         <v>10</v>
@@ -2372,7 +2370,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B42" s="2">
         <v>11</v>
@@ -2383,7 +2381,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B43" s="2">
         <v>12</v>
@@ -2394,7 +2392,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B44" s="2">
         <v>13</v>
@@ -2405,7 +2403,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B45" s="2">
         <v>14</v>
@@ -2416,7 +2414,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B46" s="2">
         <v>15</v>
@@ -2427,7 +2425,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
@@ -2438,7 +2436,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2">
         <v>2</v>
@@ -2449,7 +2447,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B49" s="2">
         <v>3</v>
@@ -2460,7 +2458,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B50" s="2">
         <v>4</v>
@@ -2471,7 +2469,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B51" s="2">
         <v>5</v>
@@ -2482,7 +2480,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B52" s="2">
         <v>6</v>
@@ -2493,7 +2491,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B53" s="2">
         <v>7</v>
@@ -2504,7 +2502,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B54" s="2">
         <v>8</v>
@@ -2515,7 +2513,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B55" s="2">
         <v>9</v>
@@ -2526,7 +2524,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B56" s="2">
         <v>10</v>
@@ -2537,7 +2535,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B57" s="2">
         <v>11</v>
@@ -2548,7 +2546,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B58" s="2">
         <v>12</v>
@@ -2559,7 +2557,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B59" s="2">
         <v>13</v>
@@ -2570,7 +2568,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B60" s="2">
         <v>14</v>
@@ -2581,7 +2579,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B61" s="2">
         <v>15</v>
@@ -2592,7 +2590,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B62" s="2">
         <v>1</v>
@@ -2603,7 +2601,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B63" s="2">
         <v>2</v>
@@ -2614,7 +2612,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B64" s="2">
         <v>3</v>
@@ -2625,7 +2623,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B65" s="2">
         <v>4</v>
@@ -2636,7 +2634,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B66" s="2">
         <v>5</v>
@@ -2647,7 +2645,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B67" s="2">
         <v>6</v>
@@ -2658,7 +2656,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B68" s="2">
         <v>7</v>
@@ -2669,7 +2667,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B69" s="2">
         <v>8</v>
@@ -2680,7 +2678,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B70" s="2">
         <v>9</v>
@@ -2691,7 +2689,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B71" s="2">
         <v>10</v>
@@ -2702,7 +2700,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B72" s="2">
         <v>11</v>
@@ -2713,7 +2711,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B73" s="2">
         <v>12</v>
@@ -2724,7 +2722,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B74" s="2">
         <v>13</v>
@@ -2735,7 +2733,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B75" s="2">
         <v>14</v>
@@ -2746,7 +2744,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B76" s="2">
         <v>15</v>
@@ -2905,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DFD714-AC29-42AA-8B1F-B5A89C9F2D11}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2917,19 +2915,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2943,10 +2941,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2960,10 +2958,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2977,10 +2975,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2994,10 +2992,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3009,27 +3007,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C387D6A-246C-42DA-928C-B6EA7B0B5C1A}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>60</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>80</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -3062,7 +3062,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>120</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>140</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>160</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>180</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>200</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>220</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>240</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>260</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>280</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>300</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>320</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>340</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>360</v>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>380</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>400</v>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>420</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>440</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>460</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>480</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>500</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>520</v>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B26">
         <v>540</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>560</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>580</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>600</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>60</v>
@@ -3348,7 +3348,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>80</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>100</v>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>120</v>
@@ -3381,7 +3381,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>140</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>160</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>180</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>200</v>
@@ -3425,7 +3425,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B38">
         <v>220</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>240</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <v>260</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B41">
         <v>280</v>
@@ -3469,7 +3469,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B42">
         <v>300</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B43">
         <v>320</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B44">
         <v>340</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>360</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B46">
         <v>380</v>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B47">
         <v>400</v>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B48">
         <v>420</v>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B49">
         <v>440</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B50">
         <v>460</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B51">
         <v>480</v>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B52">
         <v>500</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B53">
         <v>520</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B54">
         <v>540</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B55">
         <v>560</v>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>580</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B57">
         <v>600</v>
@@ -3661,18 +3661,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>210</v>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>220</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>230</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>240</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>250</v>
@@ -3739,7 +3739,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>260</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>270</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>280</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>290</v>
@@ -3783,7 +3783,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>300</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>310</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>320</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>330</v>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>340</v>
@@ -3838,7 +3838,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>350</v>
@@ -3849,7 +3849,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>360</v>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>370</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>380</v>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>390</v>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>400</v>
@@ -3904,7 +3904,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>200</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>210</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>220</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>230</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27">
         <v>240</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28">
         <v>250</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29">
         <v>260</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30">
         <v>270</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31">
         <v>280</v>
@@ -4003,7 +4003,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B32">
         <v>290</v>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33">
         <v>300</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B34">
         <v>310</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B35">
         <v>320</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36">
         <v>330</v>
@@ -4058,7 +4058,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37">
         <v>340</v>
@@ -4069,7 +4069,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38">
         <v>350</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>360</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40">
         <v>370</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>380</v>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42">
         <v>390</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43">
         <v>400</v>
@@ -4152,18 +4152,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7">
         <v>8.6343038916171701E-3</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>6.1100000000000002E-2</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>5.5599999999999997E-2</v>

</xml_diff>